<commit_message>
phone number field updated contact us page
</commit_message>
<xml_diff>
--- a/ecommerse_automation_gurupreeth/project_documents_shilpa_contactUs.xlsx
+++ b/ecommerse_automation_gurupreeth/project_documents_shilpa_contactUs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="316">
   <si>
     <t>header elements</t>
   </si>
@@ -943,6 +943,33 @@
   </si>
   <si>
     <t>http://localhost:5173/contact-us</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Shilpa</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>nshilpamurthy@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hi hello </t>
   </si>
 </sst>
 </file>
@@ -2263,40 +2290,91 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="90.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>304</v>
       </c>
       <c r="B1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>305</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>306</v>
+      </c>
+      <c r="C2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="F2">
+        <v>7483067146</v>
+      </c>
+      <c r="G2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>312</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="F3">
+        <v>7483067146</v>
+      </c>
+      <c r="G3" t="s">
+        <v>315</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>